<commit_message>
Added month filtering, but need to work on ordered by entry date instead of ID, and need to add all entries
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Downloads/inventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD90AA53-6372-074F-B39E-1CF66C749F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2451DFB1-BB64-DA4B-B24B-4C32A687A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Feature</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Bug in Current Balance…</t>
+  </si>
+  <si>
+    <t>Make sure we don't allow negative entry and to have the balance to negative</t>
+  </si>
+  <si>
+    <t>Get entries by month filter</t>
   </si>
 </sst>
 </file>
@@ -180,19 +186,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -537,7 +543,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:H17"/>
+      <selection activeCell="I15" sqref="I15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,64 +556,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -622,11 +628,11 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -639,11 +645,11 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -656,11 +662,11 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -675,11 +681,11 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -692,11 +698,11 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -711,11 +717,11 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -730,11 +736,11 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -747,19 +753,19 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -770,8 +776,10 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -779,12 +787,16 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="I14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -792,9 +804,11 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="I15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
@@ -1019,26 +1033,58 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
     <mergeCell ref="E31:H31"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="A5:D5"/>
@@ -1055,58 +1101,26 @@
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="E30:H30"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A1:K3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prevented adding entry where sale is more than the stock.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2451DFB1-BB64-DA4B-B24B-4C32A687A4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C30CE9-E806-C048-81EB-71A254B69F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Feature</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Get entries by month filter</t>
+  </si>
+  <si>
+    <t>Get All entries for a product and sort by entry date</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:K15"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,7 +762,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -771,7 +774,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -793,7 +796,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -804,14 +807,16 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+      <c r="I15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -819,9 +824,11 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="I16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>

</xml_diff>

<commit_message>
Added remove button to remove entry
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C30CE9-E806-C048-81EB-71A254B69F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C775F62-1641-BB41-9EFA-0ACCD547C28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -546,7 +546,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="I14" sqref="I14:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,11 +790,11 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="I14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">

</xml_diff>

<commit_message>
Fixed bug issue on data saving in db
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8E2352-AAC6-C14D-A836-77B0A1AE2F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A200546-95BD-8442-843F-5C9446A5A91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Feature</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Create a login page for the user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create an admin page for editing a product </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create an admin page for deleting a product 			</t>
   </si>
 </sst>
 </file>
@@ -195,22 +201,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -554,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0BDE78-032C-F845-BDC2-417C7E602CE2}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="106" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="106" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,131 +574,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="2" t="s">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="2" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
@@ -700,16 +706,16 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
         <v>11</v>
       </c>
@@ -717,156 +723,156 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="2" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="2" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="2" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="2" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="2" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="2" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="5" t="s">
         <v>11</v>
       </c>
@@ -874,213 +880,253 @@
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+    <row r="20" spans="1:11" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
     <mergeCell ref="E31:H31"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="A5:D5"/>
@@ -1097,58 +1143,26 @@
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="E30:H30"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A1:K3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added add product, product list functionality
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A200546-95BD-8442-843F-5C9446A5A91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4F2033-65DB-204C-81CB-959D89A7FA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -560,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0BDE78-032C-F845-BDC2-417C7E602CE2}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="106" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="106" workbookViewId="0">
       <selection activeCell="I21" sqref="I21:K21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added edit product functionality. Still in progress.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4F2033-65DB-204C-81CB-959D89A7FA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4909D24-0597-CC48-A5E9-BB2246A30A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Feature</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create an admin page for deleting a product 			</t>
+  </si>
+  <si>
+    <t>Refactor code for professionality</t>
   </si>
 </sst>
 </file>
@@ -201,22 +204,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -560,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0BDE78-032C-F845-BDC2-417C7E602CE2}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="106" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:K21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -574,131 +577,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
@@ -706,16 +709,16 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="5" t="s">
         <v>11</v>
       </c>
@@ -723,173 +726,173 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="5" t="s">
         <v>11</v>
       </c>
@@ -897,16 +900,16 @@
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="62" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="5" t="s">
         <v>11</v>
       </c>
@@ -914,191 +917,219 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="5" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A1:K3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
     <mergeCell ref="I31:K31"/>
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="E5:H5"/>
@@ -1115,54 +1146,30 @@
     <mergeCell ref="I28:K28"/>
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="I30:K30"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added static login signup pages, as well as some modifications. Need to implement spring security next update and the login/siggup
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE40E10D-44B1-F042-9652-36E1FC09CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8612A2BB-3549-5C4D-B37F-5FB7BB6957BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0BDE78-032C-F845-BDC2-417C7E602CE2}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="106" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Used th fragments for reusable html components
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8612A2BB-3549-5C4D-B37F-5FB7BB6957BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27416AFF-8DEF-BE41-BCE6-D7F323DA7287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Feature</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Refactor code for professionality</t>
+  </si>
+  <si>
+    <t>Add to Books functionality</t>
   </si>
 </sst>
 </file>
@@ -204,22 +207,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -563,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0BDE78-032C-F845-BDC2-417C7E602CE2}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="106" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,131 +580,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
       <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
@@ -709,16 +712,16 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="5" t="s">
         <v>11</v>
       </c>
@@ -726,173 +729,173 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
       <c r="I19" s="5" t="s">
         <v>11</v>
       </c>
@@ -900,208 +903,244 @@
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="62" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="86" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
       <c r="I22" s="5" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
+    <row r="23" spans="1:11" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
     <mergeCell ref="E31:H31"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="A5:D5"/>
@@ -1118,58 +1157,26 @@
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="E30:H30"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A1:K3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added back show message and clear mssage function inventory.js
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amieldelosreyes/Desktop/inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27416AFF-8DEF-BE41-BCE6-D7F323DA7287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA73859E-BF25-024B-B789-38576495ADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{8A5A0A2A-B7BF-E847-A036-4D503DF2CA00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Feature</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Add to Books functionality</t>
+  </si>
+  <si>
+    <t>Add Damaged Goods option</t>
   </si>
 </sst>
 </file>
@@ -207,22 +210,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -566,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0BDE78-032C-F845-BDC2-417C7E602CE2}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23:K23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="106" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,131 +583,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
@@ -712,16 +715,16 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="5" t="s">
         <v>11</v>
       </c>
@@ -729,173 +732,173 @@
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="5" t="s">
         <v>11</v>
       </c>
@@ -903,50 +906,50 @@
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="62" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="86" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="5" t="s">
         <v>11</v>
       </c>
@@ -954,165 +957,193 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+    <row r="24" spans="1:11" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A1:K3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
     <mergeCell ref="I31:K31"/>
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="E5:H5"/>
@@ -1129,54 +1160,30 @@
     <mergeCell ref="I28:K28"/>
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="I30:K30"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>